<commit_message>
feat: update jupyter notebook analisys and graphs
</commit_message>
<xml_diff>
--- a/analytics/data/fga-eps-mds-2021_1-Multilind-ANALYSYS.xlsx
+++ b/analytics/data/fga-eps-mds-2021_1-Multilind-ANALYSYS.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,42 +466,37 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>repository</t>
+          <t>Maintainability</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>version</t>
+          <t>Reliability</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>ncloc</t>
+          <t>Total_QR</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>code_quality</t>
+          <t>LOC</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>testing_status</t>
+          <t>Repository</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Maintainability</t>
+          <t>Version</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Reliability</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>total</t>
+          <t>Data</t>
         </is>
       </c>
     </row>
@@ -524,33 +519,32 @@
       <c r="F2" t="n">
         <v>1</v>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G2" t="n">
+        <v>0.2505555555555555</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.7505555555555555</v>
+      </c>
+      <c r="J2" t="n">
+        <v>322</v>
+      </c>
+      <c r="K2" t="inlineStr">
         <is>
           <t>Admin</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>2021-10-18-01.33</t>
         </is>
       </c>
-      <c r="I2" t="n">
-        <v>322</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.5011111111111111</v>
-      </c>
-      <c r="K2" t="n">
-        <v>1</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0.2505555555555555</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0.7505555555555555</v>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>2021-10-18-01.33</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -572,38 +566,37 @@
       <c r="F3" t="n">
         <v>1</v>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="G3" t="n">
+        <v>0.2762790697674419</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.7762790697674419</v>
+      </c>
+      <c r="J3" t="n">
+        <v>708</v>
+      </c>
+      <c r="K3" t="inlineStr">
         <is>
           <t>Admin</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>2021-11-04-00.35</t>
         </is>
       </c>
-      <c r="I3" t="n">
-        <v>708</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.5525581395348838</v>
-      </c>
-      <c r="K3" t="n">
-        <v>1</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0.2762790697674419</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0.7762790697674419</v>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>2021-11-04-00.35</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.625</v>
+        <v>0.7037037037037037</v>
       </c>
       <c r="B4" t="n">
         <v>0</v>
@@ -620,33 +613,32 @@
       <c r="F4" t="n">
         <v>1</v>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>User</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>2021-09-14-03:28</t>
-        </is>
+      <c r="G4" t="n">
+        <v>0.2811111111111111</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.5</v>
       </c>
       <c r="I4" t="n">
-        <v>70</v>
+        <v>0.7811111111111111</v>
       </c>
       <c r="J4" t="n">
-        <v>0.53625</v>
-      </c>
-      <c r="K4" t="n">
-        <v>1</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.268125</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0.7681249999999999</v>
+        <v>1051</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>2021-11-08-03.34</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>2021-11-08-03.34</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -668,81 +660,79 @@
       <c r="F5" t="n">
         <v>1</v>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="G5" t="n">
+        <v>0.268125</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.7681249999999999</v>
+      </c>
+      <c r="J5" t="n">
+        <v>70</v>
+      </c>
+      <c r="K5" t="inlineStr">
         <is>
           <t>User</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>2021-09-27-02.31</t>
-        </is>
-      </c>
-      <c r="I5" t="n">
-        <v>70</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0.53625</v>
-      </c>
-      <c r="K5" t="n">
-        <v>1</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.268125</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0.7681249999999999</v>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>2021-09-14-03:28</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>2021-09-14-03:28</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.5</v>
+        <v>0.625</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9285714285714286</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9285714285714286</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9285714285714286</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9285714285714286</v>
-      </c>
-      <c r="G6" t="inlineStr">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.268125</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.7681249999999999</v>
+      </c>
+      <c r="J6" t="n">
+        <v>70</v>
+      </c>
+      <c r="K6" t="inlineStr">
         <is>
           <t>User</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>2021-10-24-19.18</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>685</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.4714285714285714</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.9285714285714286</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.2357142857142857</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0.4642857142857143</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0.7</v>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>2021-09-27-02.31</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>2021-09-27-02.31</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -764,326 +754,319 @@
       <c r="F7" t="n">
         <v>0.9285714285714286</v>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="G7" t="n">
+        <v>0.2357142857142857</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.4642857142857143</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="J7" t="n">
+        <v>685</v>
+      </c>
+      <c r="K7" t="inlineStr">
         <is>
           <t>User</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>2021-11-03-22:59</t>
-        </is>
-      </c>
-      <c r="I7" t="n">
-        <v>688</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.4714285714285714</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.9285714285714286</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.2357142857142857</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0.4642857142857143</v>
-      </c>
-      <c r="N7" t="n">
-        <v>0.7</v>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>2021-10-24-19.18</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>2021-10-24-19.18</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.7142857142857143</v>
+        <v>0.5</v>
       </c>
       <c r="B8" t="n">
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>0.8928571428571429</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="D8" t="n">
-        <v>0.8928571428571429</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="E8" t="n">
-        <v>0.8928571428571429</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="F8" t="n">
-        <v>0.8928571428571429</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Content</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>2021-09-14-03:28</t>
-        </is>
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.2357142857142857</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.4642857142857143</v>
       </c>
       <c r="I8" t="n">
-        <v>629</v>
+        <v>0.7</v>
       </c>
       <c r="J8" t="n">
-        <v>0.5303571428571429</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.8928571428571428</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0.2651785714285714</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0.4464285714285714</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0.7116071428571429</v>
+        <v>688</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>User</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>2021-11-03-22:59</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>2021-11-03-22:59</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.7115384615384616</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="B9" t="n">
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0.9423076923076923</v>
+        <v>0.8928571428571429</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9423076923076923</v>
+        <v>0.8928571428571429</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9423076923076923</v>
+        <v>0.8928571428571429</v>
       </c>
       <c r="F9" t="n">
-        <v>0.9423076923076923</v>
-      </c>
-      <c r="G9" t="inlineStr">
+        <v>0.8928571428571429</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.2651785714285714</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.4464285714285714</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.7116071428571429</v>
+      </c>
+      <c r="J9" t="n">
+        <v>629</v>
+      </c>
+      <c r="K9" t="inlineStr">
         <is>
           <t>Content</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>2021-09-27-03.22</t>
-        </is>
-      </c>
-      <c r="I9" t="n">
-        <v>1323</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0.5457692307692308</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0.9423076923076923</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0.2728846153846154</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0.4711538461538461</v>
-      </c>
-      <c r="N9" t="n">
-        <v>0.7440384615384615</v>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>2021-09-14-03:28</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>2021-09-14-03:28</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.7230769230769231</v>
+        <v>0.7115384615384616</v>
       </c>
       <c r="B10" t="n">
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>0.9692307692307692</v>
+        <v>0.9423076923076923</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9692307692307692</v>
+        <v>0.9423076923076923</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9692307692307692</v>
+        <v>0.9423076923076923</v>
       </c>
       <c r="F10" t="n">
-        <v>0.9692307692307692</v>
-      </c>
-      <c r="G10" t="inlineStr">
+        <v>0.9423076923076923</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.2728846153846154</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.4711538461538461</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.7440384615384615</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1323</v>
+      </c>
+      <c r="K10" t="inlineStr">
         <is>
           <t>Content</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>2021-10-06-19.24</t>
-        </is>
-      </c>
-      <c r="I10" t="n">
-        <v>1879</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0.5584615384615385</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0.9692307692307692</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0.2792307692307692</v>
-      </c>
-      <c r="M10" t="n">
-        <v>0.4846153846153846</v>
-      </c>
-      <c r="N10" t="n">
-        <v>0.7638461538461538</v>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>2021-09-27-03.22</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>2021-09-27-03.22</t>
+        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.6979166666666666</v>
+        <v>0.7230769230769231</v>
       </c>
       <c r="B11" t="n">
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>0.9791666666666666</v>
+        <v>0.9692307692307692</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9791666666666666</v>
+        <v>0.9692307692307692</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9791666666666666</v>
+        <v>0.9692307692307692</v>
       </c>
       <c r="F11" t="n">
-        <v>0.9791666666666666</v>
-      </c>
-      <c r="G11" t="inlineStr">
+        <v>0.9692307692307692</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.2792307692307692</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.4846153846153846</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.7638461538461538</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1879</v>
+      </c>
+      <c r="K11" t="inlineStr">
         <is>
           <t>Content</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>2021-10-19-18.48</t>
-        </is>
-      </c>
-      <c r="I11" t="n">
-        <v>2477</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0.5534375</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0.9791666666666665</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0.27671875</v>
-      </c>
-      <c r="M11" t="n">
-        <v>0.4895833333333333</v>
-      </c>
-      <c r="N11" t="n">
-        <v>0.7663020833333333</v>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>2021-10-06-19.24</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>2021-10-06-19.24</t>
+        </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.71</v>
+        <v>0.6979166666666666</v>
       </c>
       <c r="B12" t="n">
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>0.98</v>
+        <v>0.9791666666666666</v>
       </c>
       <c r="D12" t="n">
-        <v>0.98</v>
+        <v>0.9791666666666666</v>
       </c>
       <c r="E12" t="n">
-        <v>0.98</v>
+        <v>0.9791666666666666</v>
       </c>
       <c r="F12" t="n">
-        <v>0.98</v>
-      </c>
-      <c r="G12" t="inlineStr">
+        <v>0.9791666666666666</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.27671875</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.4895833333333333</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.7663020833333333</v>
+      </c>
+      <c r="J12" t="n">
+        <v>2477</v>
+      </c>
+      <c r="K12" t="inlineStr">
         <is>
           <t>Content</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>2021-11-03-22:59</t>
-        </is>
-      </c>
-      <c r="I12" t="n">
-        <v>2647</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0.5577000000000001</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0.98</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0.27885</v>
-      </c>
-      <c r="M12" t="n">
-        <v>0.49</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0.76885</v>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>2021-10-19-18.48</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>2021-10-19-18.48</t>
+        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.5714285714285714</v>
+        <v>0.71</v>
       </c>
       <c r="B13" t="n">
         <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="F13" t="n">
-        <v>1</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>Files</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>2021-09-14-03:28</t>
-        </is>
+        <v>0.98</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.27885</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.49</v>
       </c>
       <c r="I13" t="n">
-        <v>54</v>
+        <v>0.76885</v>
       </c>
       <c r="J13" t="n">
-        <v>0.5185714285714286</v>
-      </c>
-      <c r="K13" t="n">
-        <v>1</v>
-      </c>
-      <c r="L13" t="n">
-        <v>0.2592857142857143</v>
-      </c>
-      <c r="M13" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="N13" t="n">
-        <v>0.7592857142857143</v>
+        <v>2647</v>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Content</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>2021-11-03-22:59</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>2021-11-03-22:59</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.5</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="B14" t="n">
         <v>0</v>
@@ -1100,33 +1083,32 @@
       <c r="F14" t="n">
         <v>1</v>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="G14" t="n">
+        <v>0.2592857142857143</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.7592857142857143</v>
+      </c>
+      <c r="J14" t="n">
+        <v>54</v>
+      </c>
+      <c r="K14" t="inlineStr">
         <is>
           <t>Files</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>2021-10-15-19.42</t>
-        </is>
-      </c>
-      <c r="I14" t="n">
-        <v>125</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0.495</v>
-      </c>
-      <c r="K14" t="n">
-        <v>1</v>
-      </c>
-      <c r="L14" t="n">
-        <v>0.2475</v>
-      </c>
-      <c r="M14" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="N14" t="n">
-        <v>0.7475000000000001</v>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>2021-09-14-03:28</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>2021-09-14-03:28</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -1148,33 +1130,32 @@
       <c r="F15" t="n">
         <v>1</v>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="G15" t="n">
+        <v>0.2475</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.7475000000000001</v>
+      </c>
+      <c r="J15" t="n">
+        <v>125</v>
+      </c>
+      <c r="K15" t="inlineStr">
         <is>
           <t>Files</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>2021-10-15-20.05</t>
-        </is>
-      </c>
-      <c r="I15" t="n">
-        <v>125</v>
-      </c>
-      <c r="J15" t="n">
-        <v>0.495</v>
-      </c>
-      <c r="K15" t="n">
-        <v>1</v>
-      </c>
-      <c r="L15" t="n">
-        <v>0.2475</v>
-      </c>
-      <c r="M15" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="N15" t="n">
-        <v>0.7475000000000001</v>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>2021-10-15-19.42</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>2021-10-15-19.42</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -1196,38 +1177,37 @@
       <c r="F16" t="n">
         <v>1</v>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="G16" t="n">
+        <v>0.2475</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.7475000000000001</v>
+      </c>
+      <c r="J16" t="n">
+        <v>125</v>
+      </c>
+      <c r="K16" t="inlineStr">
         <is>
           <t>Files</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>2021-11-03-22:59</t>
-        </is>
-      </c>
-      <c r="I16" t="n">
-        <v>132</v>
-      </c>
-      <c r="J16" t="n">
-        <v>0.495</v>
-      </c>
-      <c r="K16" t="n">
-        <v>1</v>
-      </c>
-      <c r="L16" t="n">
-        <v>0.2475</v>
-      </c>
-      <c r="M16" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="N16" t="n">
-        <v>0.7475000000000001</v>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>2021-10-15-20.05</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>2021-10-15-20.05</t>
+        </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.5</v>
       </c>
       <c r="B17" t="n">
         <v>0</v>
@@ -1244,33 +1224,32 @@
       <c r="F17" t="n">
         <v>1</v>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>Mobile_App</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>2021-09-14-03:28</t>
-        </is>
+      <c r="G17" t="n">
+        <v>0.2475</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.5</v>
       </c>
       <c r="I17" t="n">
-        <v>50</v>
+        <v>0.7475000000000001</v>
       </c>
       <c r="J17" t="n">
-        <v>0.5133333333333334</v>
-      </c>
-      <c r="K17" t="n">
-        <v>1</v>
-      </c>
-      <c r="L17" t="n">
-        <v>0.2566666666666667</v>
-      </c>
-      <c r="M17" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="N17" t="n">
-        <v>0.7566666666666667</v>
+        <v>132</v>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Files</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>2021-11-03-22:59</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>2021-11-03-22:59</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -1292,38 +1271,37 @@
       <c r="F18" t="n">
         <v>1</v>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="G18" t="n">
+        <v>0.2566666666666667</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.7566666666666667</v>
+      </c>
+      <c r="J18" t="n">
+        <v>50</v>
+      </c>
+      <c r="K18" t="inlineStr">
         <is>
           <t>Mobile_App</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>2021-09-27-03.13</t>
-        </is>
-      </c>
-      <c r="I18" t="n">
-        <v>50</v>
-      </c>
-      <c r="J18" t="n">
-        <v>0.5133333333333334</v>
-      </c>
-      <c r="K18" t="n">
-        <v>1</v>
-      </c>
-      <c r="L18" t="n">
-        <v>0.2566666666666667</v>
-      </c>
-      <c r="M18" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="N18" t="n">
-        <v>0.7566666666666667</v>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>2021-09-14-03:28</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>2021-09-14-03:28</t>
+        </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.5411764705882353</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="B19" t="n">
         <v>0</v>
@@ -1340,33 +1318,32 @@
       <c r="F19" t="n">
         <v>1</v>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="G19" t="n">
+        <v>0.2566666666666667</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.7566666666666667</v>
+      </c>
+      <c r="J19" t="n">
+        <v>50</v>
+      </c>
+      <c r="K19" t="inlineStr">
         <is>
           <t>Mobile_App</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>2021-10-19-18.47</t>
-        </is>
-      </c>
-      <c r="I19" t="n">
-        <v>2342</v>
-      </c>
-      <c r="J19" t="n">
-        <v>0.5085882352941177</v>
-      </c>
-      <c r="K19" t="n">
-        <v>1</v>
-      </c>
-      <c r="L19" t="n">
-        <v>0.2542941176470588</v>
-      </c>
-      <c r="M19" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="N19" t="n">
-        <v>0.7542941176470588</v>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>2021-09-27-03.13</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>2021-09-27-03.13</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -1388,33 +1365,126 @@
       <c r="F20" t="n">
         <v>1</v>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="G20" t="n">
+        <v>0.2542941176470588</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.7542941176470588</v>
+      </c>
+      <c r="J20" t="n">
+        <v>2342</v>
+      </c>
+      <c r="K20" t="inlineStr">
         <is>
           <t>Mobile_App</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>2021-10-19-18.47</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>2021-10-19-18.47</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>0.5411764705882353</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.2542941176470588</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.7542941176470588</v>
+      </c>
+      <c r="J21" t="n">
+        <v>2222</v>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Mobile_App</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
         <is>
           <t>2021-11-03-22:59</t>
         </is>
       </c>
-      <c r="I20" t="n">
-        <v>2222</v>
-      </c>
-      <c r="J20" t="n">
-        <v>0.5085882352941177</v>
-      </c>
-      <c r="K20" t="n">
-        <v>1</v>
-      </c>
-      <c r="L20" t="n">
-        <v>0.2542941176470588</v>
-      </c>
-      <c r="M20" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="N20" t="n">
-        <v>0.7542941176470588</v>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>2021-11-03-22:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>0.5402298850574713</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.2541379310344828</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.7541379310344828</v>
+      </c>
+      <c r="J22" t="n">
+        <v>2340</v>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Mobile_App</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>2021-11-08-20.15</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>2021-11-08-20.15</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: finish notebook analisys
</commit_message>
<xml_diff>
--- a/analytics/data/fga-eps-mds-2021_1-Multilind-ANALYSYS.xlsx
+++ b/analytics/data/fga-eps-mds-2021_1-Multilind-ANALYSYS.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1066,54 +1066,54 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.5714285714285714</v>
+        <v>0.7032967032967034</v>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>0.02197802197802198</v>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>0.978021978021978</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>0.978021978021978</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>0.978021978021978</v>
       </c>
       <c r="F14" t="n">
-        <v>1</v>
+        <v>0.978021978021978</v>
       </c>
       <c r="G14" t="n">
-        <v>0.2592857142857143</v>
+        <v>0.281043956043956</v>
       </c>
       <c r="H14" t="n">
-        <v>0.5</v>
+        <v>0.4890109890109889</v>
       </c>
       <c r="I14" t="n">
-        <v>0.7592857142857143</v>
+        <v>0.770054945054945</v>
       </c>
       <c r="J14" t="n">
-        <v>54</v>
+        <v>2038</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Files</t>
+          <t>Content</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>2021-09-14-03:28</t>
+          <t>2021-11-10-17.00</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>2021-09-14-03:28</t>
+          <t>2021-11-10-17.00</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.5</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="B15" t="n">
         <v>0</v>
@@ -1131,16 +1131,16 @@
         <v>1</v>
       </c>
       <c r="G15" t="n">
-        <v>0.2475</v>
+        <v>0.2592857142857143</v>
       </c>
       <c r="H15" t="n">
         <v>0.5</v>
       </c>
       <c r="I15" t="n">
-        <v>0.7475000000000001</v>
+        <v>0.7592857142857143</v>
       </c>
       <c r="J15" t="n">
-        <v>125</v>
+        <v>54</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>
@@ -1149,12 +1149,12 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>2021-10-15-19.42</t>
+          <t>2021-09-14-03:28</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>2021-10-15-19.42</t>
+          <t>2021-09-14-03:28</t>
         </is>
       </c>
     </row>
@@ -1196,12 +1196,12 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>2021-10-15-20.05</t>
+          <t>2021-10-15-19.42</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>2021-10-15-20.05</t>
+          <t>2021-10-15-19.42</t>
         </is>
       </c>
     </row>
@@ -1234,7 +1234,7 @@
         <v>0.7475000000000001</v>
       </c>
       <c r="J17" t="n">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="K17" t="inlineStr">
         <is>
@@ -1243,18 +1243,18 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>2021-11-03-22:59</t>
+          <t>2021-10-15-20.05</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>2021-11-03-22:59</t>
+          <t>2021-10-15-20.05</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.5</v>
       </c>
       <c r="B18" t="n">
         <v>0</v>
@@ -1272,30 +1272,30 @@
         <v>1</v>
       </c>
       <c r="G18" t="n">
-        <v>0.2566666666666667</v>
+        <v>0.2475</v>
       </c>
       <c r="H18" t="n">
         <v>0.5</v>
       </c>
       <c r="I18" t="n">
-        <v>0.7566666666666667</v>
+        <v>0.7475000000000001</v>
       </c>
       <c r="J18" t="n">
-        <v>50</v>
+        <v>132</v>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Mobile_App</t>
+          <t>Files</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>2021-09-14-03:28</t>
+          <t>2021-11-03-22:59</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>2021-09-14-03:28</t>
+          <t>2021-11-03-22:59</t>
         </is>
       </c>
     </row>
@@ -1337,18 +1337,18 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>2021-09-27-03.13</t>
+          <t>2021-09-14-03:28</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>2021-09-27-03.13</t>
+          <t>2021-09-14-03:28</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.5411764705882353</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="B20" t="n">
         <v>0</v>
@@ -1366,16 +1366,16 @@
         <v>1</v>
       </c>
       <c r="G20" t="n">
-        <v>0.2542941176470588</v>
+        <v>0.2566666666666667</v>
       </c>
       <c r="H20" t="n">
         <v>0.5</v>
       </c>
       <c r="I20" t="n">
-        <v>0.7542941176470588</v>
+        <v>0.7566666666666667</v>
       </c>
       <c r="J20" t="n">
-        <v>2342</v>
+        <v>50</v>
       </c>
       <c r="K20" t="inlineStr">
         <is>
@@ -1384,12 +1384,12 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>2021-10-19-18.47</t>
+          <t>2021-09-27-03.13</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>2021-10-19-18.47</t>
+          <t>2021-09-27-03.13</t>
         </is>
       </c>
     </row>
@@ -1422,7 +1422,7 @@
         <v>0.7542941176470588</v>
       </c>
       <c r="J21" t="n">
-        <v>2222</v>
+        <v>2342</v>
       </c>
       <c r="K21" t="inlineStr">
         <is>
@@ -1431,59 +1431,153 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>2021-11-03-22:59</t>
+          <t>2021-10-19-18.47</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>2021-11-03-22:59</t>
+          <t>2021-10-19-18.47</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
+        <v>0.5411764705882353</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.2542941176470588</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.7542941176470588</v>
+      </c>
+      <c r="J22" t="n">
+        <v>2222</v>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Mobile_App</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>2021-11-03-22:59</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>2021-11-03-22:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
         <v>0.5402298850574713</v>
       </c>
-      <c r="B22" t="n">
-        <v>0</v>
-      </c>
-      <c r="C22" t="n">
-        <v>1</v>
-      </c>
-      <c r="D22" t="n">
-        <v>1</v>
-      </c>
-      <c r="E22" t="n">
-        <v>1</v>
-      </c>
-      <c r="F22" t="n">
-        <v>1</v>
-      </c>
-      <c r="G22" t="n">
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1</v>
+      </c>
+      <c r="G23" t="n">
         <v>0.2541379310344828</v>
       </c>
-      <c r="H22" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="I22" t="n">
+      <c r="H23" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I23" t="n">
         <v>0.7541379310344828</v>
       </c>
-      <c r="J22" t="n">
+      <c r="J23" t="n">
         <v>2340</v>
       </c>
-      <c r="K22" t="inlineStr">
+      <c r="K23" t="inlineStr">
         <is>
           <t>Mobile_App</t>
         </is>
       </c>
-      <c r="L22" t="inlineStr">
+      <c r="L23" t="inlineStr">
         <is>
           <t>2021-11-08-20.15</t>
         </is>
       </c>
-      <c r="M22" t="inlineStr">
+      <c r="M23" t="inlineStr">
         <is>
           <t>2021-11-08-20.15</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>0.5444444444444444</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.2548333333333334</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.7548333333333334</v>
+      </c>
+      <c r="J24" t="n">
+        <v>2439</v>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Mobile_App</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>2021-11-10-17.28</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>2021-11-10-17.28</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: add graph labels and plot total graph
</commit_message>
<xml_diff>
--- a/analytics/data/fga-eps-mds-2021_1-Multilind-ANALYSYS.xlsx
+++ b/analytics/data/fga-eps-mds-2021_1-Multilind-ANALYSYS.xlsx
@@ -502,7 +502,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.5185185185185185</v>
+        <v>0.625</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
@@ -520,83 +520,83 @@
         <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>0.2505555555555555</v>
+        <v>0.268125</v>
       </c>
       <c r="H2" t="n">
         <v>0.5</v>
       </c>
       <c r="I2" t="n">
-        <v>0.7505555555555555</v>
+        <v>0.7681249999999999</v>
       </c>
       <c r="J2" t="n">
-        <v>322</v>
+        <v>70</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Admin</t>
+          <t>User</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2021-10-18-01.33</t>
+          <t>2021-09-14-03:28</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>2021-10-18-01.33</t>
+          <t>2021-09-14-03:28</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.6744186046511628</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="B3" t="n">
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0.8928571428571429</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0.8928571428571429</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>0.8928571428571429</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>0.8928571428571429</v>
       </c>
       <c r="G3" t="n">
-        <v>0.2762790697674419</v>
+        <v>0.2651785714285714</v>
       </c>
       <c r="H3" t="n">
-        <v>0.5</v>
+        <v>0.4464285714285714</v>
       </c>
       <c r="I3" t="n">
-        <v>0.7762790697674419</v>
+        <v>0.7116071428571429</v>
       </c>
       <c r="J3" t="n">
-        <v>708</v>
+        <v>629</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Admin</t>
+          <t>Content</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>2021-11-04-00.35</t>
+          <t>2021-09-14-03:28</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>2021-11-04-00.35</t>
+          <t>2021-09-14-03:28</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.7037037037037037</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="B4" t="n">
         <v>0</v>
@@ -614,36 +614,36 @@
         <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>0.2811111111111111</v>
+        <v>0.2566666666666667</v>
       </c>
       <c r="H4" t="n">
         <v>0.5</v>
       </c>
       <c r="I4" t="n">
-        <v>0.7811111111111111</v>
+        <v>0.7566666666666667</v>
       </c>
       <c r="J4" t="n">
-        <v>1051</v>
+        <v>50</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Admin</t>
+          <t>Mobile_App</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>2021-11-08-03.34</t>
+          <t>2021-09-14-03:28</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>2021-11-08-03.34</t>
+          <t>2021-09-14-03:28</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.625</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
@@ -661,20 +661,20 @@
         <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>0.268125</v>
+        <v>0.2592857142857143</v>
       </c>
       <c r="H5" t="n">
         <v>0.5</v>
       </c>
       <c r="I5" t="n">
-        <v>0.7681249999999999</v>
+        <v>0.7592857142857143</v>
       </c>
       <c r="J5" t="n">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>User</t>
+          <t>Files</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -737,128 +737,128 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.5</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="B7" t="n">
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9285714285714286</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9285714285714286</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9285714285714286</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>0.9285714285714286</v>
+        <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>0.2357142857142857</v>
+        <v>0.2566666666666667</v>
       </c>
       <c r="H7" t="n">
-        <v>0.4642857142857143</v>
+        <v>0.5</v>
       </c>
       <c r="I7" t="n">
-        <v>0.7</v>
+        <v>0.7566666666666667</v>
       </c>
       <c r="J7" t="n">
-        <v>685</v>
+        <v>50</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>User</t>
+          <t>Mobile_App</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>2021-10-24-19.18</t>
+          <t>2021-09-27-03.13</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>2021-10-24-19.18</t>
+          <t>2021-09-27-03.13</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.5</v>
+        <v>0.7115384615384616</v>
       </c>
       <c r="B8" t="n">
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9285714285714286</v>
+        <v>0.9423076923076923</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9285714285714286</v>
+        <v>0.9423076923076923</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9285714285714286</v>
+        <v>0.9423076923076923</v>
       </c>
       <c r="F8" t="n">
-        <v>0.9285714285714286</v>
+        <v>0.9423076923076923</v>
       </c>
       <c r="G8" t="n">
-        <v>0.2357142857142857</v>
+        <v>0.2728846153846154</v>
       </c>
       <c r="H8" t="n">
-        <v>0.4642857142857143</v>
+        <v>0.4711538461538461</v>
       </c>
       <c r="I8" t="n">
-        <v>0.7</v>
+        <v>0.7440384615384615</v>
       </c>
       <c r="J8" t="n">
-        <v>688</v>
+        <v>1323</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>User</t>
+          <t>Content</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>2021-11-03-22:59</t>
+          <t>2021-09-27-03.22</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>2021-11-03-22:59</t>
+          <t>2021-09-27-03.22</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.7142857142857143</v>
+        <v>0.7230769230769231</v>
       </c>
       <c r="B9" t="n">
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0.8928571428571429</v>
+        <v>0.9692307692307692</v>
       </c>
       <c r="D9" t="n">
-        <v>0.8928571428571429</v>
+        <v>0.9692307692307692</v>
       </c>
       <c r="E9" t="n">
-        <v>0.8928571428571429</v>
+        <v>0.9692307692307692</v>
       </c>
       <c r="F9" t="n">
-        <v>0.8928571428571429</v>
+        <v>0.9692307692307692</v>
       </c>
       <c r="G9" t="n">
-        <v>0.2651785714285714</v>
+        <v>0.2792307692307692</v>
       </c>
       <c r="H9" t="n">
-        <v>0.4464285714285714</v>
+        <v>0.4846153846153846</v>
       </c>
       <c r="I9" t="n">
-        <v>0.7116071428571429</v>
+        <v>0.7638461538461538</v>
       </c>
       <c r="J9" t="n">
-        <v>629</v>
+        <v>1879</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
@@ -867,233 +867,233 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>2021-09-14-03:28</t>
+          <t>2021-10-06-19.24</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>2021-09-14-03:28</t>
+          <t>2021-10-06-19.24</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.7115384615384616</v>
+        <v>0.5</v>
       </c>
       <c r="B10" t="n">
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>0.9423076923076923</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9423076923076923</v>
+        <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9423076923076923</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
-        <v>0.9423076923076923</v>
+        <v>1</v>
       </c>
       <c r="G10" t="n">
-        <v>0.2728846153846154</v>
+        <v>0.2475</v>
       </c>
       <c r="H10" t="n">
-        <v>0.4711538461538461</v>
+        <v>0.5</v>
       </c>
       <c r="I10" t="n">
-        <v>0.7440384615384615</v>
+        <v>0.7475000000000001</v>
       </c>
       <c r="J10" t="n">
-        <v>1323</v>
+        <v>125</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Content</t>
+          <t>Files</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>2021-09-27-03.22</t>
+          <t>2021-10-15-19.42</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>2021-09-27-03.22</t>
+          <t>2021-10-15-19.42</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.7230769230769231</v>
+        <v>0.5</v>
       </c>
       <c r="B11" t="n">
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>0.9692307692307692</v>
+        <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9692307692307692</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9692307692307692</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>0.9692307692307692</v>
+        <v>1</v>
       </c>
       <c r="G11" t="n">
-        <v>0.2792307692307692</v>
+        <v>0.2475</v>
       </c>
       <c r="H11" t="n">
-        <v>0.4846153846153846</v>
+        <v>0.5</v>
       </c>
       <c r="I11" t="n">
-        <v>0.7638461538461538</v>
+        <v>0.7475000000000001</v>
       </c>
       <c r="J11" t="n">
-        <v>1879</v>
+        <v>125</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Content</t>
+          <t>Files</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>2021-10-06-19.24</t>
+          <t>2021-10-15-20.05</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>2021-10-06-19.24</t>
+          <t>2021-10-15-20.05</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.6979166666666666</v>
+        <v>0.5185185185185185</v>
       </c>
       <c r="B12" t="n">
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>0.9791666666666666</v>
+        <v>1</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9791666666666666</v>
+        <v>1</v>
       </c>
       <c r="E12" t="n">
-        <v>0.9791666666666666</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
-        <v>0.9791666666666666</v>
+        <v>1</v>
       </c>
       <c r="G12" t="n">
-        <v>0.27671875</v>
+        <v>0.2505555555555555</v>
       </c>
       <c r="H12" t="n">
-        <v>0.4895833333333333</v>
+        <v>0.5</v>
       </c>
       <c r="I12" t="n">
-        <v>0.7663020833333333</v>
+        <v>0.7505555555555555</v>
       </c>
       <c r="J12" t="n">
-        <v>2477</v>
+        <v>322</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Content</t>
+          <t>Admin</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>2021-10-19-18.48</t>
+          <t>2021-10-18-01.33</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>2021-10-19-18.48</t>
+          <t>2021-10-18-01.33</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.71</v>
+        <v>0.5411764705882353</v>
       </c>
       <c r="B13" t="n">
         <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="D13" t="n">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="E13" t="n">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="F13" t="n">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="G13" t="n">
-        <v>0.27885</v>
+        <v>0.2542941176470588</v>
       </c>
       <c r="H13" t="n">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="I13" t="n">
-        <v>0.76885</v>
+        <v>0.7542941176470588</v>
       </c>
       <c r="J13" t="n">
-        <v>2647</v>
+        <v>2342</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Content</t>
+          <t>Mobile_App</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>2021-11-03-22:59</t>
+          <t>2021-10-19-18.47</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>2021-11-03-22:59</t>
+          <t>2021-10-19-18.47</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.7032967032967034</v>
+        <v>0.6979166666666666</v>
       </c>
       <c r="B14" t="n">
-        <v>0.02197802197802198</v>
+        <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>0.978021978021978</v>
+        <v>0.9791666666666666</v>
       </c>
       <c r="D14" t="n">
-        <v>0.978021978021978</v>
+        <v>0.9791666666666666</v>
       </c>
       <c r="E14" t="n">
-        <v>0.978021978021978</v>
+        <v>0.9791666666666666</v>
       </c>
       <c r="F14" t="n">
-        <v>0.978021978021978</v>
+        <v>0.9791666666666666</v>
       </c>
       <c r="G14" t="n">
-        <v>0.281043956043956</v>
+        <v>0.27671875</v>
       </c>
       <c r="H14" t="n">
-        <v>0.4890109890109889</v>
+        <v>0.4895833333333333</v>
       </c>
       <c r="I14" t="n">
-        <v>0.770054945054945</v>
+        <v>0.7663020833333333</v>
       </c>
       <c r="J14" t="n">
-        <v>2038</v>
+        <v>2477</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
@@ -1102,65 +1102,65 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>2021-11-10-17.00</t>
+          <t>2021-10-19-18.48</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>2021-11-10-17.00</t>
+          <t>2021-10-19-18.48</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.5714285714285714</v>
+        <v>0.5</v>
       </c>
       <c r="B15" t="n">
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="F15" t="n">
-        <v>1</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="G15" t="n">
-        <v>0.2592857142857143</v>
+        <v>0.2357142857142857</v>
       </c>
       <c r="H15" t="n">
-        <v>0.5</v>
+        <v>0.4642857142857143</v>
       </c>
       <c r="I15" t="n">
-        <v>0.7592857142857143</v>
+        <v>0.7</v>
       </c>
       <c r="J15" t="n">
-        <v>54</v>
+        <v>685</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Files</t>
+          <t>User</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>2021-09-14-03:28</t>
+          <t>2021-10-24-19.18</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>2021-09-14-03:28</t>
+          <t>2021-10-24-19.18</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.5</v>
+        <v>0.5411764705882353</v>
       </c>
       <c r="B16" t="n">
         <v>0</v>
@@ -1178,30 +1178,30 @@
         <v>1</v>
       </c>
       <c r="G16" t="n">
-        <v>0.2475</v>
+        <v>0.2542941176470588</v>
       </c>
       <c r="H16" t="n">
         <v>0.5</v>
       </c>
       <c r="I16" t="n">
-        <v>0.7475000000000001</v>
+        <v>0.7542941176470588</v>
       </c>
       <c r="J16" t="n">
-        <v>125</v>
+        <v>2222</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Files</t>
+          <t>Mobile_App</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>2021-10-15-19.42</t>
+          <t>2021-11-03-22:59</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>2021-10-15-19.42</t>
+          <t>2021-11-03-22:59</t>
         </is>
       </c>
     </row>
@@ -1234,7 +1234,7 @@
         <v>0.7475000000000001</v>
       </c>
       <c r="J17" t="n">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="K17" t="inlineStr">
         <is>
@@ -1243,49 +1243,49 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>2021-10-15-20.05</t>
+          <t>2021-11-03-22:59</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>2021-10-15-20.05</t>
+          <t>2021-11-03-22:59</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.5</v>
+        <v>0.71</v>
       </c>
       <c r="B18" t="n">
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="D18" t="n">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="F18" t="n">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="G18" t="n">
-        <v>0.2475</v>
+        <v>0.27885</v>
       </c>
       <c r="H18" t="n">
-        <v>0.5</v>
+        <v>0.49</v>
       </c>
       <c r="I18" t="n">
-        <v>0.7475000000000001</v>
+        <v>0.76885</v>
       </c>
       <c r="J18" t="n">
-        <v>132</v>
+        <v>2647</v>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Files</t>
+          <t>Content</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1301,54 +1301,54 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.5</v>
       </c>
       <c r="B19" t="n">
         <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="F19" t="n">
-        <v>1</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="G19" t="n">
-        <v>0.2566666666666667</v>
+        <v>0.2357142857142857</v>
       </c>
       <c r="H19" t="n">
-        <v>0.5</v>
+        <v>0.4642857142857143</v>
       </c>
       <c r="I19" t="n">
-        <v>0.7566666666666667</v>
+        <v>0.7</v>
       </c>
       <c r="J19" t="n">
-        <v>50</v>
+        <v>688</v>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Mobile_App</t>
+          <t>User</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>2021-09-14-03:28</t>
+          <t>2021-11-03-22:59</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>2021-09-14-03:28</t>
+          <t>2021-11-03-22:59</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.6744186046511628</v>
       </c>
       <c r="B20" t="n">
         <v>0</v>
@@ -1366,36 +1366,36 @@
         <v>1</v>
       </c>
       <c r="G20" t="n">
-        <v>0.2566666666666667</v>
+        <v>0.2762790697674419</v>
       </c>
       <c r="H20" t="n">
         <v>0.5</v>
       </c>
       <c r="I20" t="n">
-        <v>0.7566666666666667</v>
+        <v>0.7762790697674419</v>
       </c>
       <c r="J20" t="n">
-        <v>50</v>
+        <v>708</v>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Mobile_App</t>
+          <t>Admin</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>2021-09-27-03.13</t>
+          <t>2021-11-04-00.35</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>2021-09-27-03.13</t>
+          <t>2021-11-04-00.35</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.5411764705882353</v>
+        <v>0.7037037037037037</v>
       </c>
       <c r="B21" t="n">
         <v>0</v>
@@ -1413,36 +1413,36 @@
         <v>1</v>
       </c>
       <c r="G21" t="n">
-        <v>0.2542941176470588</v>
+        <v>0.2811111111111111</v>
       </c>
       <c r="H21" t="n">
         <v>0.5</v>
       </c>
       <c r="I21" t="n">
-        <v>0.7542941176470588</v>
+        <v>0.7811111111111111</v>
       </c>
       <c r="J21" t="n">
-        <v>2342</v>
+        <v>1051</v>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Mobile_App</t>
+          <t>Admin</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>2021-10-19-18.47</t>
+          <t>2021-11-08-03.34</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>2021-10-19-18.47</t>
+          <t>2021-11-08-03.34</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.5411764705882353</v>
+        <v>0.5402298850574713</v>
       </c>
       <c r="B22" t="n">
         <v>0</v>
@@ -1460,16 +1460,16 @@
         <v>1</v>
       </c>
       <c r="G22" t="n">
-        <v>0.2542941176470588</v>
+        <v>0.2541379310344828</v>
       </c>
       <c r="H22" t="n">
         <v>0.5</v>
       </c>
       <c r="I22" t="n">
-        <v>0.7542941176470588</v>
+        <v>0.7541379310344828</v>
       </c>
       <c r="J22" t="n">
-        <v>2222</v>
+        <v>2340</v>
       </c>
       <c r="K22" t="inlineStr">
         <is>
@@ -1478,59 +1478,59 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>2021-11-03-22:59</t>
+          <t>2021-11-08-20.15</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>2021-11-03-22:59</t>
+          <t>2021-11-08-20.15</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.5402298850574713</v>
+        <v>0.7032967032967034</v>
       </c>
       <c r="B23" t="n">
-        <v>0</v>
+        <v>0.02197802197802198</v>
       </c>
       <c r="C23" t="n">
-        <v>1</v>
+        <v>0.978021978021978</v>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>0.978021978021978</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>0.978021978021978</v>
       </c>
       <c r="F23" t="n">
-        <v>1</v>
+        <v>0.978021978021978</v>
       </c>
       <c r="G23" t="n">
-        <v>0.2541379310344828</v>
+        <v>0.281043956043956</v>
       </c>
       <c r="H23" t="n">
-        <v>0.5</v>
+        <v>0.4890109890109889</v>
       </c>
       <c r="I23" t="n">
-        <v>0.7541379310344828</v>
+        <v>0.770054945054945</v>
       </c>
       <c r="J23" t="n">
-        <v>2340</v>
+        <v>2038</v>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Mobile_App</t>
+          <t>Content</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>2021-11-08-20.15</t>
+          <t>2021-11-10-17.00</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>2021-11-08-20.15</t>
+          <t>2021-11-10-17.00</t>
         </is>
       </c>
     </row>

</xml_diff>